<commit_message>
updated the samples table
</commit_message>
<xml_diff>
--- a/data/samples.xlsx
+++ b/data/samples.xlsx
@@ -5,27 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gonev\Lynx\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gonev\Lynx\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5F0646-68BA-4553-9C82-2D7EC1B1B225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08519C44-AA1D-4174-A345-7E12D3D93805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="186">
   <si>
     <t>c_ll_ca_0240</t>
   </si>
@@ -304,13 +316,292 @@
   </si>
   <si>
     <t>Used in IntroScan</t>
+  </si>
+  <si>
+    <t>c_ll_ba_0224</t>
+  </si>
+  <si>
+    <t>c_ll_ba_0226</t>
+  </si>
+  <si>
+    <t>c_ll_ba_0227</t>
+  </si>
+  <si>
+    <t>c_ll_ba_0228</t>
+  </si>
+  <si>
+    <t>c_ll_ba_0229</t>
+  </si>
+  <si>
+    <t>c_ll_ba_0230</t>
+  </si>
+  <si>
+    <t>c_ll_ba_0233</t>
+  </si>
+  <si>
+    <t>c_ll_ca_0249</t>
+  </si>
+  <si>
+    <t>c_ll_ca_0253</t>
+  </si>
+  <si>
+    <t>c_ll_cr_0205</t>
+  </si>
+  <si>
+    <t>c_ll_cr_0206</t>
+  </si>
+  <si>
+    <t>c_ll_cr_0207</t>
+  </si>
+  <si>
+    <t>c_ll_cr_0208</t>
+  </si>
+  <si>
+    <t>c_ll_cr_0209</t>
+  </si>
+  <si>
+    <t>c_ll_cr_0211</t>
+  </si>
+  <si>
+    <t>c_ll_cr_0212</t>
+  </si>
+  <si>
+    <t>c_ll_ka_0184</t>
+  </si>
+  <si>
+    <t>c_ll_ka_0186</t>
+  </si>
+  <si>
+    <t>c_ll_ka_0188</t>
+  </si>
+  <si>
+    <t>c_ll_ka_0189</t>
+  </si>
+  <si>
+    <t>c_ll_la_0044</t>
+  </si>
+  <si>
+    <t>c_ll_la_0045</t>
+  </si>
+  <si>
+    <t>c_ll_la_0047</t>
+  </si>
+  <si>
+    <t>c_ll_la_0048</t>
+  </si>
+  <si>
+    <t>c_ll_la_0052</t>
+  </si>
+  <si>
+    <t>c_ll_la_0053</t>
+  </si>
+  <si>
+    <t>c_ll_la_0054</t>
+  </si>
+  <si>
+    <t>c_ll_no_0065</t>
+  </si>
+  <si>
+    <t>c_ll_no_0075</t>
+  </si>
+  <si>
+    <t>c_ll_no_0076</t>
+  </si>
+  <si>
+    <t>c_ll_no_0077</t>
+  </si>
+  <si>
+    <t>c_ll_no_0078</t>
+  </si>
+  <si>
+    <t>c_ll_no_0079</t>
+  </si>
+  <si>
+    <t>c_ll_no_0080</t>
+  </si>
+  <si>
+    <t>c_ll_no_0081</t>
+  </si>
+  <si>
+    <t>c_ll_no_0082</t>
+  </si>
+  <si>
+    <t>c_ll_og_0181</t>
+  </si>
+  <si>
+    <t>c_ll_og_0187</t>
+  </si>
+  <si>
+    <t>c_ll_po_0001</t>
+  </si>
+  <si>
+    <t>c_ll_po_0002</t>
+  </si>
+  <si>
+    <t>c_ll_po_0003</t>
+  </si>
+  <si>
+    <t>c_ll_po_0011</t>
+  </si>
+  <si>
+    <t>c_ll_po_0014</t>
+  </si>
+  <si>
+    <t>c_ll_po_0019</t>
+  </si>
+  <si>
+    <t>c_ll_po_0105</t>
+  </si>
+  <si>
+    <t>c_ll_po_0106</t>
+  </si>
+  <si>
+    <t>c_ll_po_0150</t>
+  </si>
+  <si>
+    <t>c_ll_to_0190</t>
+  </si>
+  <si>
+    <t>c_ll_to_0191</t>
+  </si>
+  <si>
+    <t>c_ll_tu_0153</t>
+  </si>
+  <si>
+    <t>c_ll_tu_0154</t>
+  </si>
+  <si>
+    <t>c_ll_tu_0157</t>
+  </si>
+  <si>
+    <t>c_ll_tu_0158</t>
+  </si>
+  <si>
+    <t>c_ll_tu_0159</t>
+  </si>
+  <si>
+    <t>c_ll_tu_0165</t>
+  </si>
+  <si>
+    <t>c_ll_tu_0166</t>
+  </si>
+  <si>
+    <t>Subspecies</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>X coord</t>
+  </si>
+  <si>
+    <t>Y coord</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Coverage depth</t>
+  </si>
+  <si>
+    <t>Used in GEA</t>
+  </si>
+  <si>
+    <t>Balkans</t>
+  </si>
+  <si>
+    <t>L. l. balcanicus</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Caucasus</t>
+  </si>
+  <si>
+    <t>L. l. dinniki</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Carpathians</t>
+  </si>
+  <si>
+    <t>L. l. carpathicus</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>L. l. wrangeli</t>
+  </si>
+  <si>
+    <t>Kirov</t>
+  </si>
+  <si>
+    <t>L. l. lynx</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>North-Eastern Poland</t>
+  </si>
+  <si>
+    <t>Tuva</t>
+  </si>
+  <si>
+    <t>Urals</t>
+  </si>
+  <si>
+    <t>Primosky Krai</t>
+  </si>
+  <si>
+    <t>Yakutia</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +629,25 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -359,11 +669,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,15 +974,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
@@ -2014,6 +2344,3836 @@
         <v>6</v>
       </c>
     </row>
+    <row r="53" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="5"/>
+    </row>
+    <row r="94" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="5"/>
+    </row>
+    <row r="98" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="5"/>
+      <c r="H99" s="5"/>
+    </row>
+    <row r="100" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+    </row>
+    <row r="101" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="5"/>
+      <c r="G101" s="5"/>
+      <c r="H101" s="5"/>
+    </row>
+    <row r="102" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="5"/>
+      <c r="G102" s="5"/>
+      <c r="H102" s="5"/>
+    </row>
+    <row r="103" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+    </row>
+    <row r="104" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+    </row>
+    <row r="105" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+    </row>
+    <row r="106" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="5"/>
+    </row>
+    <row r="107" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+    </row>
+    <row r="108" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C67BD5A0-7202-4DFA-89B5-3DECE745ED1D}">
+  <dimension ref="A1:I108"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.5546875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="7">
+        <v>20.77</v>
+      </c>
+      <c r="F2" s="7">
+        <v>41.48</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="9">
+        <v>31.7</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="7">
+        <v>20.96</v>
+      </c>
+      <c r="F3" s="7">
+        <v>41.5</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H3" s="9">
+        <v>14.71</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="7">
+        <v>20.82</v>
+      </c>
+      <c r="F4" s="7">
+        <v>41.38</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="9">
+        <v>16.48</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="7">
+        <v>20.94</v>
+      </c>
+      <c r="F5" s="7">
+        <v>41.63</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H5" s="9">
+        <v>27.24</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="7">
+        <v>20.79</v>
+      </c>
+      <c r="F6" s="7">
+        <v>41.48</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" s="9">
+        <v>21.33</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="7">
+        <v>20.79</v>
+      </c>
+      <c r="F7" s="7">
+        <v>41.48</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="9">
+        <v>19.91</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H8" s="9">
+        <v>21.5</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="7">
+        <v>42.49</v>
+      </c>
+      <c r="F9" s="7">
+        <v>41.46</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H9" s="9">
+        <v>34.6</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" s="7">
+        <v>46.38</v>
+      </c>
+      <c r="F10" s="7">
+        <v>41.87</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H10" s="9">
+        <v>21.96</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="7">
+        <v>44.93</v>
+      </c>
+      <c r="F11" s="7">
+        <v>40.03</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" s="9">
+        <v>22.11</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="7">
+        <v>47.84</v>
+      </c>
+      <c r="F12" s="7">
+        <v>41.57</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H12" s="9">
+        <v>27.3</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="7">
+        <v>47.89</v>
+      </c>
+      <c r="F13" s="7">
+        <v>41.73</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" s="9">
+        <v>18.16</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="7">
+        <v>46.67</v>
+      </c>
+      <c r="F14" s="7">
+        <v>42.39</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="9">
+        <v>8.49</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E15" s="7">
+        <v>44.35</v>
+      </c>
+      <c r="F15" s="7">
+        <v>41.69</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="9">
+        <v>13.07</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="7">
+        <v>42.81</v>
+      </c>
+      <c r="F16" s="7">
+        <v>43.04</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" s="9">
+        <v>11.3</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" s="7">
+        <v>43.25</v>
+      </c>
+      <c r="F17" s="7">
+        <v>43.2</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" s="9">
+        <v>16.91</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E18" s="7">
+        <v>42.06</v>
+      </c>
+      <c r="F18" s="7">
+        <v>41.57</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H18" s="9">
+        <v>14.45</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="7">
+        <v>46.39</v>
+      </c>
+      <c r="F19" s="7">
+        <v>42.69</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H19" s="9">
+        <v>12.3</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E20" s="7">
+        <v>46.45</v>
+      </c>
+      <c r="F20" s="7">
+        <v>42.1</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H20" s="9">
+        <v>16.72</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="7">
+        <v>19.760000000000002</v>
+      </c>
+      <c r="F21" s="7">
+        <v>49.67</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H21" s="9">
+        <v>8.17</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" s="7">
+        <v>25.6</v>
+      </c>
+      <c r="F22" s="7">
+        <v>45.64</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H22" s="9">
+        <v>7.86</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" s="7">
+        <v>22.2</v>
+      </c>
+      <c r="F23" s="7">
+        <v>45.4</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="9">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E24" s="7">
+        <v>22.3</v>
+      </c>
+      <c r="F24" s="7">
+        <v>49.75</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H24" s="9">
+        <v>7.82</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" s="7">
+        <v>22.2</v>
+      </c>
+      <c r="F25" s="7">
+        <v>45.4</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H25" s="9">
+        <v>8.84</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H26" s="9">
+        <v>24.02</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E27" s="7">
+        <v>22.43</v>
+      </c>
+      <c r="F27" s="7">
+        <v>49.71</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H27" s="9">
+        <v>19.88</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" s="7">
+        <v>108.64</v>
+      </c>
+      <c r="F28" s="7">
+        <v>48.38</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H28" s="9">
+        <v>7.3</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" s="7">
+        <v>108.07</v>
+      </c>
+      <c r="F29" s="7">
+        <v>48.41</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H29" s="9">
+        <v>7.01</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E30" s="7">
+        <v>110.49</v>
+      </c>
+      <c r="F30" s="7">
+        <v>48.62</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H30" s="9">
+        <v>6.31</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" s="7">
+        <v>110.5</v>
+      </c>
+      <c r="F31" s="7">
+        <v>49.62</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H31" s="9">
+        <v>6.26</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E32" s="7">
+        <v>101.05</v>
+      </c>
+      <c r="F32" s="7">
+        <v>43.23</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" s="9">
+        <v>7.08</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="7">
+        <v>103.78</v>
+      </c>
+      <c r="F33" s="7">
+        <v>48.64</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H33" s="9">
+        <v>5.85</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" s="7">
+        <v>108.27</v>
+      </c>
+      <c r="F34" s="7">
+        <v>47.4</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="9">
+        <v>7.58</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E35" s="7">
+        <v>108.68</v>
+      </c>
+      <c r="F35" s="7">
+        <v>47.63</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H35" s="9">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="7">
+        <v>50.4</v>
+      </c>
+      <c r="F36" s="7">
+        <v>59.81</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H36" s="9">
+        <v>21.68</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="7">
+        <v>50.4</v>
+      </c>
+      <c r="F37" s="7">
+        <v>59.81</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H37" s="9">
+        <v>6.31</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" s="7">
+        <v>50.4</v>
+      </c>
+      <c r="F38" s="7">
+        <v>59.81</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H38" s="9">
+        <v>5.37</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E39" s="7">
+        <v>50.4</v>
+      </c>
+      <c r="F39" s="7">
+        <v>59.81</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H39" s="9">
+        <v>5.46</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="7">
+        <v>50.4</v>
+      </c>
+      <c r="F40" s="7">
+        <v>59.81</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H40" s="9">
+        <v>6.06</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="7">
+        <v>48.42</v>
+      </c>
+      <c r="F41" s="7">
+        <v>60.81</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H41" s="9">
+        <v>5.52</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="7">
+        <v>48.42</v>
+      </c>
+      <c r="F42" s="7">
+        <v>60.81</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H42" s="9">
+        <v>6.37</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="7">
+        <v>48.42</v>
+      </c>
+      <c r="F43" s="7">
+        <v>60.81</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H43" s="9">
+        <v>6.12</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="7">
+        <v>48.42</v>
+      </c>
+      <c r="F44" s="7">
+        <v>60.81</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" s="9">
+        <v>5.88</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="7">
+        <v>48.42</v>
+      </c>
+      <c r="F45" s="7">
+        <v>60.81</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" s="9">
+        <v>6.1</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="7">
+        <v>46.73</v>
+      </c>
+      <c r="F46" s="7">
+        <v>61.19</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H46" s="9">
+        <v>6.42</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E47" s="7">
+        <v>46.73</v>
+      </c>
+      <c r="F47" s="7">
+        <v>61.19</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H47" s="9">
+        <v>6.38</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E48" s="7">
+        <v>46.73</v>
+      </c>
+      <c r="F48" s="7">
+        <v>61.19</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H48" s="9">
+        <v>6.34</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E49" s="7">
+        <v>22.53</v>
+      </c>
+      <c r="F49" s="7">
+        <v>56.64</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H49" s="9">
+        <v>7.76</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" s="7">
+        <v>27.58</v>
+      </c>
+      <c r="F50" s="7">
+        <v>56.31</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H50" s="9">
+        <v>23.97</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E51" s="7">
+        <v>28.15</v>
+      </c>
+      <c r="F51" s="7">
+        <v>56.38</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H51" s="9">
+        <v>7.02</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E52" s="7">
+        <v>22.82</v>
+      </c>
+      <c r="F52" s="7">
+        <v>57.36</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H52" s="9">
+        <v>5.2</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E53" s="7">
+        <v>22.6</v>
+      </c>
+      <c r="F53" s="7">
+        <v>57.35</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H53" s="9">
+        <v>6.74</v>
+      </c>
+      <c r="I53" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E54" s="7">
+        <v>22.82</v>
+      </c>
+      <c r="F54" s="7">
+        <v>57.05</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H54" s="9">
+        <v>7.67</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" s="7">
+        <v>25.57</v>
+      </c>
+      <c r="F55" s="7">
+        <v>57.67</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H55" s="9">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E56" s="7">
+        <v>21.34</v>
+      </c>
+      <c r="F56" s="7">
+        <v>69.510000000000005</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H56" s="9">
+        <v>22.98</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E57" s="7">
+        <v>12.36</v>
+      </c>
+      <c r="F57" s="7">
+        <v>64.510000000000005</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H57" s="9">
+        <v>5.59</v>
+      </c>
+      <c r="I57" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E58" s="7">
+        <v>10.68</v>
+      </c>
+      <c r="F58" s="7">
+        <v>63.82</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H58" s="9">
+        <v>6</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E59" s="7">
+        <v>10.95</v>
+      </c>
+      <c r="F59" s="7">
+        <v>63.57</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H59" s="9">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E60" s="7">
+        <v>12.15</v>
+      </c>
+      <c r="F60" s="7">
+        <v>61.38</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H60" s="9">
+        <v>5.39</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E61" s="7">
+        <v>8.41</v>
+      </c>
+      <c r="F61" s="7">
+        <v>59.4</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H61" s="9">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E62" s="7">
+        <v>8.73</v>
+      </c>
+      <c r="F62" s="7">
+        <v>60.66</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H62" s="9">
+        <v>5.3</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E63" s="7">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="F63" s="7">
+        <v>60.27</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H63" s="9">
+        <v>5.59</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E64" s="7">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="F64" s="7">
+        <v>60.14</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H64" s="9">
+        <v>5.51</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E65" s="7">
+        <v>23.6</v>
+      </c>
+      <c r="F65" s="7">
+        <v>52.95</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H65" s="9">
+        <v>6.73</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E66" s="7">
+        <v>23.84</v>
+      </c>
+      <c r="F66" s="7">
+        <v>52.82</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H66" s="9">
+        <v>6.67</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E67" s="7">
+        <v>23.72</v>
+      </c>
+      <c r="F67" s="7">
+        <v>52.8</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H67" s="9">
+        <v>6.49</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E68" s="7">
+        <v>23.51</v>
+      </c>
+      <c r="F68" s="7">
+        <v>52.89</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H68" s="9">
+        <v>6.61</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E69" s="7">
+        <v>23.95</v>
+      </c>
+      <c r="F69" s="7">
+        <v>52.77</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H69" s="9">
+        <v>6.61</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E70" s="7">
+        <v>23.74</v>
+      </c>
+      <c r="F70" s="7">
+        <v>52.68</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H70" s="9">
+        <v>6.59</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E71" s="7">
+        <v>23.47</v>
+      </c>
+      <c r="F71" s="7">
+        <v>53.09</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H71" s="9">
+        <v>5.44</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E72" s="7">
+        <v>23.66</v>
+      </c>
+      <c r="F72" s="7">
+        <v>53.1</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H72" s="9">
+        <v>5.76</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E73" s="7">
+        <v>23.6</v>
+      </c>
+      <c r="F73" s="7">
+        <v>52.76</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H73" s="9">
+        <v>23.99</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E74" s="7">
+        <v>96.53</v>
+      </c>
+      <c r="F74" s="7">
+        <v>51.48</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H74" s="9">
+        <v>8.25</v>
+      </c>
+      <c r="I74" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E75" s="7">
+        <v>96.53</v>
+      </c>
+      <c r="F75" s="7">
+        <v>51.48</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H75" s="9">
+        <v>22.02</v>
+      </c>
+      <c r="I75" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E76" s="7">
+        <v>96.53</v>
+      </c>
+      <c r="F76" s="7">
+        <v>51.48</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H76" s="9">
+        <v>8.16</v>
+      </c>
+      <c r="I76" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E77" s="7">
+        <v>96.53</v>
+      </c>
+      <c r="F77" s="7">
+        <v>51.48</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H77" s="9">
+        <v>8.15</v>
+      </c>
+      <c r="I77" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E78" s="7">
+        <v>96.53</v>
+      </c>
+      <c r="F78" s="7">
+        <v>51.48</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H78" s="9">
+        <v>7.91</v>
+      </c>
+      <c r="I78" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E79" s="7">
+        <v>96.53</v>
+      </c>
+      <c r="F79" s="7">
+        <v>51.48</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H79" s="9">
+        <v>7.88</v>
+      </c>
+      <c r="I79" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E80" s="7">
+        <v>96.53</v>
+      </c>
+      <c r="F80" s="7">
+        <v>51.48</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H80" s="9">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="I80" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E81" s="7">
+        <v>59.64</v>
+      </c>
+      <c r="F81" s="7">
+        <v>56.05</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H81" s="9">
+        <v>11.29</v>
+      </c>
+      <c r="I81" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A82" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E82" s="7">
+        <v>60.13</v>
+      </c>
+      <c r="F82" s="7">
+        <v>55.15</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H82" s="9">
+        <v>12.27</v>
+      </c>
+      <c r="I82" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A83" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E83" s="7">
+        <v>60.13</v>
+      </c>
+      <c r="F83" s="7">
+        <v>55.15</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H83" s="9">
+        <v>12.91</v>
+      </c>
+      <c r="I83" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E84" s="7">
+        <v>59.79</v>
+      </c>
+      <c r="F84" s="7">
+        <v>55.18</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H84" s="9">
+        <v>13.83</v>
+      </c>
+      <c r="I84" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A85" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E85" s="7">
+        <v>59</v>
+      </c>
+      <c r="F85" s="7">
+        <v>55</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H85" s="9">
+        <v>13.33</v>
+      </c>
+      <c r="I85" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A86" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E86" s="7">
+        <v>60.89</v>
+      </c>
+      <c r="F86" s="7">
+        <v>54.38</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H86" s="9">
+        <v>23.47</v>
+      </c>
+      <c r="I86" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E87" s="7">
+        <v>57.36</v>
+      </c>
+      <c r="F87" s="7">
+        <v>55</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H87" s="9">
+        <v>13.79</v>
+      </c>
+      <c r="I87" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A88" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E88" s="7">
+        <v>136.47</v>
+      </c>
+      <c r="F88" s="7">
+        <v>44.94</v>
+      </c>
+      <c r="G88" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H88" s="9">
+        <v>6.54</v>
+      </c>
+      <c r="I88" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A89" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E89" s="7">
+        <v>135.58000000000001</v>
+      </c>
+      <c r="F89" s="7">
+        <v>45.29</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H89" s="9">
+        <v>11.58</v>
+      </c>
+      <c r="I89" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A90" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E90" s="7">
+        <v>136.72999999999999</v>
+      </c>
+      <c r="F90" s="7">
+        <v>45.67</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H90" s="9">
+        <v>5.94</v>
+      </c>
+      <c r="I90" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E91" s="7">
+        <v>132.91</v>
+      </c>
+      <c r="F91" s="7">
+        <v>49.01</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H91" s="9">
+        <v>7.08</v>
+      </c>
+      <c r="I91" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E92" s="7">
+        <v>137.01</v>
+      </c>
+      <c r="F92" s="7">
+        <v>45.86</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H92" s="9">
+        <v>29.33</v>
+      </c>
+      <c r="I92" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E93" s="7">
+        <v>137.01</v>
+      </c>
+      <c r="F93" s="7">
+        <v>45.86</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H93" s="9">
+        <v>8.75</v>
+      </c>
+      <c r="I93" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A94" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E94" s="7">
+        <v>137.61000000000001</v>
+      </c>
+      <c r="F94" s="7">
+        <v>47.29</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H94" s="9">
+        <v>23.4</v>
+      </c>
+      <c r="I94" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A95" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E95" s="7">
+        <v>137.43</v>
+      </c>
+      <c r="F95" s="7">
+        <v>45.91</v>
+      </c>
+      <c r="G95" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H95" s="9">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="I95" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A96" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E96" s="7">
+        <v>137.43</v>
+      </c>
+      <c r="F96" s="7">
+        <v>45.91</v>
+      </c>
+      <c r="G96" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H96" s="9">
+        <v>8.66</v>
+      </c>
+      <c r="I96" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E97" s="7">
+        <v>133.46</v>
+      </c>
+      <c r="F97" s="7">
+        <v>51.39</v>
+      </c>
+      <c r="G97" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H97" s="9">
+        <v>25.47</v>
+      </c>
+      <c r="I97" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E98" s="7">
+        <v>132.07</v>
+      </c>
+      <c r="F98" s="7">
+        <v>59.9</v>
+      </c>
+      <c r="G98" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H98" s="9">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="I98" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E99" s="7">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="F99" s="7">
+        <v>61.19</v>
+      </c>
+      <c r="G99" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H99" s="9">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="I99" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E100" s="7">
+        <v>129.16</v>
+      </c>
+      <c r="F100" s="7">
+        <v>61.16</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H100" s="9">
+        <v>8.48</v>
+      </c>
+      <c r="I100" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E101" s="7">
+        <v>136.18</v>
+      </c>
+      <c r="F101" s="7">
+        <v>66.89</v>
+      </c>
+      <c r="G101" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H101" s="9">
+        <v>23.6</v>
+      </c>
+      <c r="I101" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E102" s="7">
+        <v>136.18</v>
+      </c>
+      <c r="F102" s="7">
+        <v>66.89</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H102" s="9">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="I102" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A103" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E103" s="7">
+        <v>136.18</v>
+      </c>
+      <c r="F103" s="7">
+        <v>66.89</v>
+      </c>
+      <c r="G103" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H103" s="9">
+        <v>8.14</v>
+      </c>
+      <c r="I103" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E104" s="7">
+        <v>129.44999999999999</v>
+      </c>
+      <c r="F104" s="7">
+        <v>61.89</v>
+      </c>
+      <c r="G104" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H104" s="9">
+        <v>8.59</v>
+      </c>
+      <c r="I104" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A105" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E105" s="7">
+        <v>130.68</v>
+      </c>
+      <c r="F105" s="7">
+        <v>60.78</v>
+      </c>
+      <c r="G105" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H105" s="9">
+        <v>23.58</v>
+      </c>
+      <c r="I105" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E106" s="7">
+        <v>127.3</v>
+      </c>
+      <c r="F106" s="7">
+        <v>60.75</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H106" s="9">
+        <v>8.26</v>
+      </c>
+      <c r="I106" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E107" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="G107" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H107" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I107" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E108" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="F108" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H108" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I108" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sample names and sex
</commit_message>
<xml_diff>
--- a/data/samples.xlsx
+++ b/data/samples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gonev\Lynx\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08519C44-AA1D-4174-A345-7E12D3D93805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB02BEF-23AE-4960-BEB3-58DB40AB020A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -676,24 +676,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3026,53 +3024,53 @@
   <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="16.5546875" style="4"/>
+    <col min="1" max="1" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.5546875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.5546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -3101,7 +3099,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -3130,7 +3128,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -3159,7 +3157,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -3188,7 +3186,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -3217,7 +3215,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -3246,7 +3244,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -3275,7 +3273,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -3304,7 +3302,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -3333,7 +3331,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -3362,7 +3360,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -3391,7 +3389,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -3420,7 +3418,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3449,7 +3447,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -3478,7 +3476,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -3507,7 +3505,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -3536,7 +3534,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -3565,7 +3563,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -3594,7 +3592,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -3623,7 +3621,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -3652,7 +3650,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -3681,7 +3679,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -3710,7 +3708,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -3739,7 +3737,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -3768,7 +3766,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -3797,7 +3795,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="7" t="s">
         <v>108</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -3826,7 +3824,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -3855,7 +3853,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="7" t="s">
         <v>110</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -3884,7 +3882,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -3913,7 +3911,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -3942,7 +3940,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -3971,7 +3969,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -4000,7 +3998,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="7" t="s">
         <v>140</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -4029,7 +4027,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -4058,7 +4056,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -4087,7 +4085,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -4116,7 +4114,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -4145,7 +4143,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -4174,7 +4172,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -4203,7 +4201,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -4232,7 +4230,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -4261,7 +4259,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -4290,7 +4288,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -4319,7 +4317,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -4348,7 +4346,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="7" t="s">
@@ -4377,7 +4375,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B47" s="7" t="s">
@@ -4406,7 +4404,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B48" s="7" t="s">
@@ -4435,7 +4433,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -4464,7 +4462,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="7" t="s">
         <v>114</v>
       </c>
       <c r="B50" s="7" t="s">
@@ -4493,7 +4491,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B51" s="7" t="s">
@@ -4522,7 +4520,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B52" s="7" t="s">
@@ -4551,7 +4549,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -4580,7 +4578,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B54" s="7" t="s">
@@ -4609,7 +4607,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B55" s="7" t="s">
@@ -4638,7 +4636,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="7" t="s">
         <v>120</v>
       </c>
       <c r="B56" s="7" t="s">
@@ -4667,7 +4665,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B57" s="7" t="s">
@@ -4696,7 +4694,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="7" t="s">
         <v>122</v>
       </c>
       <c r="B58" s="7" t="s">
@@ -4725,7 +4723,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="7" t="s">
         <v>123</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -4754,7 +4752,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="7" t="s">
         <v>124</v>
       </c>
       <c r="B60" s="7" t="s">
@@ -4783,7 +4781,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
+      <c r="A61" s="7" t="s">
         <v>125</v>
       </c>
       <c r="B61" s="7" t="s">
@@ -4812,7 +4810,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="7" t="s">
         <v>126</v>
       </c>
       <c r="B62" s="7" t="s">
@@ -4841,7 +4839,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="7" t="s">
         <v>127</v>
       </c>
       <c r="B63" s="7" t="s">
@@ -4870,7 +4868,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="7" t="s">
         <v>128</v>
       </c>
       <c r="B64" s="7" t="s">
@@ -4899,7 +4897,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B65" s="7" t="s">
@@ -4928,7 +4926,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="7" t="s">
         <v>132</v>
       </c>
       <c r="B66" s="7" t="s">
@@ -4957,7 +4955,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B67" s="7" t="s">
@@ -4986,7 +4984,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="7" t="s">
         <v>134</v>
       </c>
       <c r="B68" s="7" t="s">
@@ -5015,7 +5013,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="7" t="s">
         <v>135</v>
       </c>
       <c r="B69" s="7" t="s">
@@ -5044,7 +5042,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="7" t="s">
         <v>136</v>
       </c>
       <c r="B70" s="7" t="s">
@@ -5073,7 +5071,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="7" t="s">
         <v>137</v>
       </c>
       <c r="B71" s="7" t="s">
@@ -5102,7 +5100,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="7" t="s">
         <v>138</v>
       </c>
       <c r="B72" s="7" t="s">
@@ -5131,7 +5129,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="7" t="s">
         <v>139</v>
       </c>
       <c r="B73" s="7" t="s">
@@ -5160,7 +5158,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B74" s="7" t="s">
@@ -5189,7 +5187,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B75" s="7" t="s">
@@ -5218,7 +5216,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B76" s="7" t="s">
@@ -5247,7 +5245,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B77" s="7" t="s">
@@ -5276,7 +5274,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B78" s="7" t="s">
@@ -5305,7 +5303,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B79" s="7" t="s">
@@ -5334,7 +5332,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B80" s="7" t="s">
@@ -5363,7 +5361,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B81" s="7" t="s">
@@ -5392,7 +5390,7 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B82" s="7" t="s">
@@ -5421,7 +5419,7 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="10" t="s">
+      <c r="A83" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B83" s="7" t="s">
@@ -5450,7 +5448,7 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="10" t="s">
+      <c r="A84" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B84" s="7" t="s">
@@ -5479,7 +5477,7 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B85" s="7" t="s">
@@ -5508,7 +5506,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B86" s="7" t="s">
@@ -5537,7 +5535,7 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="10" t="s">
+      <c r="A87" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B87" s="7" t="s">
@@ -5566,7 +5564,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="10" t="s">
+      <c r="A88" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B88" s="7" t="s">
@@ -5595,7 +5593,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="10" t="s">
+      <c r="A89" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B89" s="7" t="s">
@@ -5624,7 +5622,7 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B90" s="7" t="s">
@@ -5653,7 +5651,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="10" t="s">
+      <c r="A91" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B91" s="7" t="s">
@@ -5682,7 +5680,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B92" s="7" t="s">
@@ -5711,7 +5709,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="10" t="s">
+      <c r="A93" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B93" s="7" t="s">
@@ -5740,7 +5738,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="10" t="s">
+      <c r="A94" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B94" s="7" t="s">
@@ -5769,7 +5767,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="10" t="s">
+      <c r="A95" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B95" s="7" t="s">
@@ -5798,7 +5796,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B96" s="7" t="s">
@@ -5827,7 +5825,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="10" t="s">
+      <c r="A97" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B97" s="7" t="s">
@@ -5856,7 +5854,7 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B98" s="7" t="s">
@@ -5885,7 +5883,7 @@
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B99" s="7" t="s">
@@ -5914,7 +5912,7 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="10" t="s">
+      <c r="A100" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B100" s="7" t="s">
@@ -5943,7 +5941,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="10" t="s">
+      <c r="A101" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B101" s="7" t="s">
@@ -5972,7 +5970,7 @@
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="10" t="s">
+      <c r="A102" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B102" s="7" t="s">
@@ -6001,7 +5999,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="10" t="s">
+      <c r="A103" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B103" s="7" t="s">
@@ -6030,7 +6028,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="10" t="s">
+      <c r="A104" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B104" s="7" t="s">
@@ -6059,7 +6057,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="10" t="s">
+      <c r="A105" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B105" s="7" t="s">
@@ -6088,7 +6086,7 @@
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="10" t="s">
+      <c r="A106" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B106" s="7" t="s">
@@ -6117,7 +6115,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="11" t="s">
         <v>100</v>
       </c>
       <c r="B107" s="7" t="s">
@@ -6126,19 +6124,19 @@
       <c r="C107" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D107" s="11" t="s">
+      <c r="D107" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E107" s="11" t="s">
+      <c r="E107" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F107" s="11" t="s">
+      <c r="F107" s="6" t="s">
         <v>185</v>
       </c>
       <c r="G107" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H107" s="11" t="s">
+      <c r="H107" s="6" t="s">
         <v>185</v>
       </c>
       <c r="I107" s="9" t="s">
@@ -6146,7 +6144,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="11" t="s">
         <v>101</v>
       </c>
       <c r="B108" s="7" t="s">
@@ -6155,19 +6153,19 @@
       <c r="C108" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D108" s="11" t="s">
+      <c r="D108" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E108" s="11" t="s">
+      <c r="E108" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="F108" s="11" t="s">
+      <c r="F108" s="6" t="s">
         <v>185</v>
       </c>
       <c r="G108" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="H108" s="11" t="s">
+      <c r="H108" s="6" t="s">
         <v>185</v>
       </c>
       <c r="I108" s="9" t="s">

</xml_diff>